<commit_message>
Update Init and Plan
</commit_message>
<xml_diff>
--- a/docs/Project_management/1_Initiate/WSM_ProjectManager_Selection.xlsx
+++ b/docs/Project_management/1_Initiate/WSM_ProjectManager_Selection.xlsx
@@ -196,12 +196,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,10 +223,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Bảng Đánh Giá Các Thành Viên</a:t>
             </a:r>
           </a:p>
@@ -236,7 +242,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.33660953852595366"/>
+          <c:x val="0.33660953852595371"/>
           <c:y val="2.470356923151153E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -247,9 +253,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14987723978162901"/>
+          <c:x val="0.14987723978162903"/>
           <c:y val="0.1449740733627809"/>
-          <c:w val="0.78173974091196419"/>
+          <c:w val="0.78173974091196408"/>
           <c:h val="0.73973903907635663"/>
         </c:manualLayout>
       </c:layout>
@@ -301,11 +307,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="70521984"/>
-        <c:axId val="70523520"/>
+        <c:axId val="80482688"/>
+        <c:axId val="80485376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70521984"/>
+        <c:axId val="80482688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,7 +328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70523520"/>
+        <c:crossAx val="80485376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -331,7 +337,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70523520"/>
+        <c:axId val="80485376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -349,7 +355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70521984"/>
+        <c:crossAx val="80482688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -359,7 +365,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -755,7 +761,7 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -770,14 +776,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="12" t="s">
@@ -872,7 +878,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3">
@@ -912,7 +918,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3">
@@ -955,19 +961,19 @@
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>0.1</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>80</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>75</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>70</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>70</v>
       </c>
     </row>

</xml_diff>